<commit_message>
split holidays codes into codes and regions
</commit_message>
<xml_diff>
--- a/docs/feriados.xlsx
+++ b/docs/feriados.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\859494\Desktop\work_related\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://galp-my.sharepoint.com/personal/859494_galp_com/Documents/Development/holidays/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_DD8E0E5D5A599FC0FF7E03DCF5B12E834BA98E30" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6FB7B9B-91B6-44C0-9412-E81891DF0F63}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="330" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2597,7 +2598,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2993,7 +2994,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G349"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
@@ -10092,7 +10093,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A289:E300">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A289:E300">
     <sortCondition ref="D289"/>
   </sortState>
   <dataConsolidate/>

</xml_diff>